<commit_message>
updated scripts to support Nodata (-1) from CSV tables and upgraded to Python 3
</commit_message>
<xml_diff>
--- a/OGC_IAU2000_WKT_v2/Source_Python/naifcodes_radii_m_wAsteroids_IAU2000.xlsx
+++ b/OGC_IAU2000_WKT_v2/Source_Python/naifcodes_radii_m_wAsteroids_IAU2000.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trent\Downloads\GDAL_scripts-master\OGC_IAU2000_WKT_v2\Source_Python\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-45" yWindow="-30" windowWidth="11580" windowHeight="12885"/>
   </bookViews>
@@ -568,7 +573,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1047,9 +1052,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1101,6 +1107,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1148,7 +1157,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1181,9 +1190,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1216,6 +1242,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1394,7 +1437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171:F178"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1913,6 +1958,18 @@
       <c r="B26" t="s">
         <v>26</v>
       </c>
+      <c r="C26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1921,6 +1978,18 @@
       <c r="B27" t="s">
         <v>27</v>
       </c>
+      <c r="C27" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1929,6 +1998,18 @@
       <c r="B28" t="s">
         <v>28</v>
       </c>
+      <c r="C28" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1937,6 +2018,18 @@
       <c r="B29" t="s">
         <v>29</v>
       </c>
+      <c r="C29" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F29" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1945,6 +2038,18 @@
       <c r="B30" t="s">
         <v>30</v>
       </c>
+      <c r="C30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F30" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1953,6 +2058,18 @@
       <c r="B31" t="s">
         <v>31</v>
       </c>
+      <c r="C31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F31" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1961,133 +2078,337 @@
       <c r="B32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F32" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>524</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>525</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>526</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F35" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>527</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>528</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>529</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F38" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>530</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E39" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F39" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>531</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E40" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F40" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>532</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E41" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F41" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>533</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F42" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>534</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E43" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>535</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E44" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>536</v>
       </c>
       <c r="B45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E45" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F45" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>537</v>
       </c>
       <c r="B46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F46" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>538</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E47" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F47" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>539</v>
       </c>
       <c r="B48" t="s">
         <v>48</v>
+      </c>
+      <c r="C48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E48" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F48" s="2">
+        <v>-1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,6 +2418,18 @@
       <c r="B49" t="s">
         <v>49</v>
       </c>
+      <c r="C49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E49" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F49" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -2105,6 +2438,18 @@
       <c r="B50" t="s">
         <v>50</v>
       </c>
+      <c r="C50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E50" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F50" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
@@ -2113,6 +2458,18 @@
       <c r="B51" t="s">
         <v>51</v>
       </c>
+      <c r="C51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E51" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F51" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -2121,6 +2478,18 @@
       <c r="B52" t="s">
         <v>52</v>
       </c>
+      <c r="C52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E52" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F52" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -2129,6 +2498,18 @@
       <c r="B53" t="s">
         <v>53</v>
       </c>
+      <c r="C53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E53" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F53" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -2137,6 +2518,18 @@
       <c r="B54" t="s">
         <v>54</v>
       </c>
+      <c r="C54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E54" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F54" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -2145,6 +2538,18 @@
       <c r="B55" t="s">
         <v>55</v>
       </c>
+      <c r="C55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E55" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F55" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -2153,6 +2558,18 @@
       <c r="B56" t="s">
         <v>56</v>
       </c>
+      <c r="C56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E56" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F56" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -2161,6 +2578,18 @@
       <c r="B57" t="s">
         <v>57</v>
       </c>
+      <c r="C57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F57" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -2169,6 +2598,18 @@
       <c r="B58" t="s">
         <v>147</v>
       </c>
+      <c r="C58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E58" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F58" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -2177,6 +2618,18 @@
       <c r="B59" t="s">
         <v>148</v>
       </c>
+      <c r="C59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E59" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F59" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -2565,6 +3018,18 @@
       <c r="B79" t="s">
         <v>77</v>
       </c>
+      <c r="C79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F79" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -2573,6 +3038,18 @@
       <c r="B80" t="s">
         <v>78</v>
       </c>
+      <c r="C80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F80" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
@@ -2581,6 +3058,18 @@
       <c r="B81" t="s">
         <v>79</v>
       </c>
+      <c r="C81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F81" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
@@ -2589,6 +3078,18 @@
       <c r="B82" t="s">
         <v>80</v>
       </c>
+      <c r="C82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F82" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
@@ -2597,6 +3098,18 @@
       <c r="B83" t="s">
         <v>81</v>
       </c>
+      <c r="C83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E83" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F83" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -2605,6 +3118,18 @@
       <c r="B84" t="s">
         <v>82</v>
       </c>
+      <c r="C84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E84" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F84" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
@@ -2613,6 +3138,18 @@
       <c r="B85" t="s">
         <v>83</v>
       </c>
+      <c r="C85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E85" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F85" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
@@ -2621,6 +3158,18 @@
       <c r="B86" t="s">
         <v>84</v>
       </c>
+      <c r="C86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E86" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F86" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
@@ -2629,6 +3178,18 @@
       <c r="B87" t="s">
         <v>85</v>
       </c>
+      <c r="C87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E87" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F87" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
@@ -2637,6 +3198,18 @@
       <c r="B88" t="s">
         <v>86</v>
       </c>
+      <c r="C88" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D88" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E88" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F88" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
@@ -2645,6 +3218,18 @@
       <c r="B89" t="s">
         <v>87</v>
       </c>
+      <c r="C89" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D89" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E89" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F89" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
@@ -2653,6 +3238,18 @@
       <c r="B90" t="s">
         <v>88</v>
       </c>
+      <c r="C90" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D90" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E90" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F90" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
@@ -2661,6 +3258,18 @@
       <c r="B91" t="s">
         <v>89</v>
       </c>
+      <c r="C91" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D91" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E91" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F91" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
@@ -2729,6 +3338,18 @@
       <c r="B95" t="s">
         <v>149</v>
       </c>
+      <c r="C95" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D95" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E95" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F95" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
@@ -2737,133 +3358,337 @@
       <c r="B96" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D96" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E96" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F96" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>637</v>
       </c>
       <c r="B97" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D97" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E97" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F97" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>638</v>
       </c>
       <c r="B98" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D98" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E98" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F98" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>639</v>
       </c>
       <c r="B99" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D99" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E99" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F99" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>640</v>
       </c>
       <c r="B100" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D100" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E100" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F100" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>641</v>
       </c>
       <c r="B101" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D101" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E101" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F101" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>642</v>
       </c>
       <c r="B102" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D102" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E102" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F102" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>643</v>
       </c>
       <c r="B103" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D103" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E103" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F103" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>644</v>
       </c>
       <c r="B104" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D104" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E104" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F104" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>645</v>
       </c>
       <c r="B105" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D105" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E105" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F105" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>646</v>
       </c>
       <c r="B106" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D106" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E106" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F106" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>647</v>
       </c>
       <c r="B107" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D107" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E107" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F107" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>648</v>
       </c>
       <c r="B108" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D108" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E108" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F108" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>649</v>
       </c>
       <c r="B109" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D109" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E109" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F109" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>650</v>
       </c>
       <c r="B110" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D110" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E110" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F110" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>651</v>
       </c>
       <c r="B111" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D111" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E111" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F111" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>652</v>
       </c>
       <c r="B112" t="s">
         <v>166</v>
+      </c>
+      <c r="C112" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D112" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E112" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F112" s="2">
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2873,6 +3698,18 @@
       <c r="B113" t="s">
         <v>167</v>
       </c>
+      <c r="C113" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D113" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E113" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F113" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
@@ -3201,6 +4038,18 @@
       <c r="B130" t="s">
         <v>108</v>
       </c>
+      <c r="C130" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D130" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E130" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F130" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
@@ -3209,6 +4058,18 @@
       <c r="B131" t="s">
         <v>109</v>
       </c>
+      <c r="C131" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D131" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E131" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F131" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
@@ -3217,6 +4078,18 @@
       <c r="B132" t="s">
         <v>110</v>
       </c>
+      <c r="C132" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D132" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E132" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F132" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
@@ -3225,6 +4098,18 @@
       <c r="B133" t="s">
         <v>111</v>
       </c>
+      <c r="C133" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D133" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E133" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F133" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
@@ -3233,6 +4118,18 @@
       <c r="B134" t="s">
         <v>112</v>
       </c>
+      <c r="C134" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D134" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E134" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F134" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
@@ -3241,6 +4138,18 @@
       <c r="B135" t="s">
         <v>113</v>
       </c>
+      <c r="C135" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D135" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E135" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F135" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
@@ -3249,6 +4158,18 @@
       <c r="B136" t="s">
         <v>168</v>
       </c>
+      <c r="C136" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D136" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E136" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F136" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
@@ -3257,6 +4178,18 @@
       <c r="B137" t="s">
         <v>169</v>
       </c>
+      <c r="C137" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D137" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E137" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F137" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
@@ -3265,6 +4198,18 @@
       <c r="B138" t="s">
         <v>170</v>
       </c>
+      <c r="C138" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D138" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E138" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F138" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
@@ -3273,6 +4218,18 @@
       <c r="B139" t="s">
         <v>171</v>
       </c>
+      <c r="C139" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D139" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E139" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F139" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
@@ -3281,6 +4238,18 @@
       <c r="B140" t="s">
         <v>172</v>
       </c>
+      <c r="C140" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D140" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E140" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F140" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
@@ -3289,6 +4258,18 @@
       <c r="B141" t="s">
         <v>173</v>
       </c>
+      <c r="C141" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D141" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E141" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F141" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
@@ -3477,6 +4458,18 @@
       <c r="B151" t="s">
         <v>174</v>
       </c>
+      <c r="C151" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D151" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E151" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F151" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
@@ -3485,6 +4478,18 @@
       <c r="B152" t="s">
         <v>175</v>
       </c>
+      <c r="C152" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D152" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E152" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F152" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
@@ -3493,6 +4498,18 @@
       <c r="B153" t="s">
         <v>176</v>
       </c>
+      <c r="C153" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D153" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E153" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F153" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
@@ -3501,6 +4518,18 @@
       <c r="B154" t="s">
         <v>177</v>
       </c>
+      <c r="C154" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D154" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E154" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F154" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
@@ -3509,6 +4538,18 @@
       <c r="B155" t="s">
         <v>178</v>
       </c>
+      <c r="C155" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D155" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E155" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F155" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
@@ -3557,6 +4598,18 @@
       <c r="B158" t="s">
         <v>182</v>
       </c>
+      <c r="C158" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D158" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E158" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F158" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
@@ -3565,6 +4618,18 @@
       <c r="B159" t="s">
         <v>180</v>
       </c>
+      <c r="C159" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D159" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E159" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F159" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
@@ -3573,6 +4638,18 @@
       <c r="B160" t="s">
         <v>181</v>
       </c>
+      <c r="C160" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D160" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E160" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F160" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
@@ -3581,6 +4658,18 @@
       <c r="B161" t="s">
         <v>179</v>
       </c>
+      <c r="C161" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D161" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E161" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F161" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
@@ -3629,6 +4718,18 @@
       <c r="B164" t="s">
         <v>128</v>
       </c>
+      <c r="C164" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D164" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E164" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F164" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
@@ -3657,6 +4758,18 @@
       <c r="B166" t="s">
         <v>130</v>
       </c>
+      <c r="C166" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D166" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E166" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F166" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
@@ -3665,6 +4778,18 @@
       <c r="B167" t="s">
         <v>131</v>
       </c>
+      <c r="C167" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D167" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E167" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F167" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
@@ -3693,6 +4818,9 @@
       <c r="B169" t="s">
         <v>133</v>
       </c>
+      <c r="C169" s="2">
+        <v>-1</v>
+      </c>
       <c r="D169" s="1">
         <v>108500</v>
       </c>
@@ -3730,6 +4858,18 @@
       <c r="B171" t="s">
         <v>135</v>
       </c>
+      <c r="C171" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D171" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E171" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F171" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
@@ -3738,6 +4878,18 @@
       <c r="B172" t="s">
         <v>136</v>
       </c>
+      <c r="C172" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D172" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E172" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F172" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
@@ -3746,6 +4898,18 @@
       <c r="B173" t="s">
         <v>137</v>
       </c>
+      <c r="C173" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D173" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E173" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F173" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
@@ -3754,6 +4918,18 @@
       <c r="B174" t="s">
         <v>125</v>
       </c>
+      <c r="C174" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D174" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E174" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F174" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
@@ -3762,6 +4938,18 @@
       <c r="B175" t="s">
         <v>138</v>
       </c>
+      <c r="C175" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D175" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E175" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F175" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
@@ -3770,21 +4958,57 @@
       <c r="B176" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D176" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E176" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F176" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2004179</v>
       </c>
       <c r="B177" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C177" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D177" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E177" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F177" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2025143</v>
       </c>
       <c r="B178" t="s">
         <v>141</v>
+      </c>
+      <c r="C178" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D178" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E178" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F178" s="2">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>